<commit_message>
Updated TC4 results Rev E
</commit_message>
<xml_diff>
--- a/Test Case - 4/TC4_Results_E.xlsx
+++ b/Test Case - 4/TC4_Results_E.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="11925"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="11925" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reductive" sheetId="1" r:id="rId1"/>
@@ -644,7 +644,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -783,6 +783,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -828,7 +841,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -873,13 +886,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -887,8 +903,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -935,27 +957,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="64">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="56">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1033,66 +1035,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1854,9 +1796,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q26" sqref="Q26"/>
+      <selection pane="bottomLeft" activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1868,48 +1810,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="15" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="15" t="s">
         <v>78</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="6" t="s">
         <v>79</v>
       </c>
@@ -1928,16 +1870,16 @@
       <c r="G2" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="17" t="s">
+      <c r="H2" s="16"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="15" t="s">
         <v>77</v>
       </c>
       <c r="P2" s="1"/>
@@ -4386,11 +4328,11 @@
       <c r="L76" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M76" s="17" t="s">
+      <c r="M76" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="N76" s="17"/>
-      <c r="O76" s="17"/>
+      <c r="N76" s="15"/>
+      <c r="O76" s="15"/>
       <c r="Q76" t="b">
         <v>1</v>
       </c>
@@ -4413,9 +4355,9 @@
       <c r="J77" s="9"/>
       <c r="K77" s="9"/>
       <c r="L77" s="9"/>
-      <c r="M77" s="17"/>
-      <c r="N77" s="17"/>
-      <c r="O77" s="17"/>
+      <c r="M77" s="15"/>
+      <c r="N77" s="15"/>
+      <c r="O77" s="15"/>
       <c r="Q77" t="b">
         <v>1</v>
       </c>
@@ -4454,9 +4396,9 @@
       <c r="L78" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M78" s="17"/>
-      <c r="N78" s="17"/>
-      <c r="O78" s="17"/>
+      <c r="M78" s="15"/>
+      <c r="N78" s="15"/>
+      <c r="O78" s="15"/>
       <c r="Q78" t="b">
         <v>1</v>
       </c>
@@ -4498,9 +4440,9 @@
       <c r="L79" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M79" s="17"/>
-      <c r="N79" s="17"/>
-      <c r="O79" s="17"/>
+      <c r="M79" s="15"/>
+      <c r="N79" s="15"/>
+      <c r="O79" s="15"/>
       <c r="Q79" t="b">
         <v>1</v>
       </c>
@@ -4542,9 +4484,9 @@
       <c r="L80" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M80" s="17"/>
-      <c r="N80" s="17"/>
-      <c r="O80" s="17"/>
+      <c r="M80" s="15"/>
+      <c r="N80" s="15"/>
+      <c r="O80" s="15"/>
       <c r="Q80" t="b">
         <v>1</v>
       </c>
@@ -4567,9 +4509,9 @@
       <c r="J81" s="11"/>
       <c r="K81" s="11"/>
       <c r="L81" s="11"/>
-      <c r="M81" s="17"/>
-      <c r="N81" s="17"/>
-      <c r="O81" s="17"/>
+      <c r="M81" s="15"/>
+      <c r="N81" s="15"/>
+      <c r="O81" s="15"/>
       <c r="Q81" t="b">
         <v>1</v>
       </c>
@@ -4608,9 +4550,9 @@
       <c r="L82" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M82" s="17"/>
-      <c r="N82" s="17"/>
-      <c r="O82" s="17"/>
+      <c r="M82" s="15"/>
+      <c r="N82" s="15"/>
+      <c r="O82" s="15"/>
       <c r="Q82" t="b">
         <v>1</v>
       </c>
@@ -4652,9 +4594,9 @@
       <c r="L83" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M83" s="17"/>
-      <c r="N83" s="17"/>
-      <c r="O83" s="17"/>
+      <c r="M83" s="15"/>
+      <c r="N83" s="15"/>
+      <c r="O83" s="15"/>
       <c r="Q83" t="b">
         <v>1</v>
       </c>
@@ -4696,9 +4638,9 @@
       <c r="L84" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M84" s="17"/>
-      <c r="N84" s="17"/>
-      <c r="O84" s="17"/>
+      <c r="M84" s="15"/>
+      <c r="N84" s="15"/>
+      <c r="O84" s="15"/>
       <c r="Q84" t="b">
         <v>1</v>
       </c>
@@ -4740,9 +4682,9 @@
       <c r="L85" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M85" s="17"/>
-      <c r="N85" s="17"/>
-      <c r="O85" s="17"/>
+      <c r="M85" s="15"/>
+      <c r="N85" s="15"/>
+      <c r="O85" s="15"/>
       <c r="Q85" t="b">
         <v>1</v>
       </c>
@@ -4765,9 +4707,9 @@
       <c r="J86" s="11"/>
       <c r="K86" s="11"/>
       <c r="L86" s="11"/>
-      <c r="M86" s="17"/>
-      <c r="N86" s="17"/>
-      <c r="O86" s="17"/>
+      <c r="M86" s="15"/>
+      <c r="N86" s="15"/>
+      <c r="O86" s="15"/>
       <c r="Q86" t="b">
         <v>1</v>
       </c>
@@ -4806,9 +4748,9 @@
       <c r="L87" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M87" s="17"/>
-      <c r="N87" s="17"/>
-      <c r="O87" s="17"/>
+      <c r="M87" s="15"/>
+      <c r="N87" s="15"/>
+      <c r="O87" s="15"/>
       <c r="Q87" t="b">
         <v>1</v>
       </c>
@@ -4850,9 +4792,9 @@
       <c r="L88" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M88" s="17"/>
-      <c r="N88" s="17"/>
-      <c r="O88" s="17"/>
+      <c r="M88" s="15"/>
+      <c r="N88" s="15"/>
+      <c r="O88" s="15"/>
       <c r="Q88" t="b">
         <v>1</v>
       </c>
@@ -5159,11 +5101,11 @@
       <c r="L95" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M95" s="17" t="s">
+      <c r="M95" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="N95" s="17"/>
-      <c r="O95" s="17"/>
+      <c r="N95" s="15"/>
+      <c r="O95" s="15"/>
       <c r="P95" s="8"/>
       <c r="Q95" t="b">
         <v>1</v>
@@ -5186,9 +5128,9 @@
       <c r="G96" s="6">
         <v>13.6</v>
       </c>
-      <c r="M96" s="17"/>
-      <c r="N96" s="17"/>
-      <c r="O96" s="17"/>
+      <c r="M96" s="15"/>
+      <c r="N96" s="15"/>
+      <c r="O96" s="15"/>
       <c r="P96" s="8"/>
       <c r="Q96" t="b">
         <v>1</v>
@@ -5232,9 +5174,9 @@
       <c r="L97" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M97" s="17"/>
-      <c r="N97" s="17"/>
-      <c r="O97" s="17"/>
+      <c r="M97" s="15"/>
+      <c r="N97" s="15"/>
+      <c r="O97" s="15"/>
       <c r="P97" s="8"/>
       <c r="Q97" t="b">
         <v>1</v>
@@ -5281,9 +5223,9 @@
       <c r="L98" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M98" s="17"/>
-      <c r="N98" s="17"/>
-      <c r="O98" s="17"/>
+      <c r="M98" s="15"/>
+      <c r="N98" s="15"/>
+      <c r="O98" s="15"/>
       <c r="P98" s="8"/>
       <c r="Q98" t="b">
         <v>1</v>
@@ -5330,9 +5272,9 @@
       <c r="L99" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M99" s="17"/>
-      <c r="N99" s="17"/>
-      <c r="O99" s="17"/>
+      <c r="M99" s="15"/>
+      <c r="N99" s="15"/>
+      <c r="O99" s="15"/>
       <c r="P99" s="8"/>
       <c r="Q99" t="b">
         <v>1</v>
@@ -5355,9 +5297,9 @@
       <c r="G100" s="6">
         <v>13.6</v>
       </c>
-      <c r="M100" s="17"/>
-      <c r="N100" s="17"/>
-      <c r="O100" s="17"/>
+      <c r="M100" s="15"/>
+      <c r="N100" s="15"/>
+      <c r="O100" s="15"/>
       <c r="P100" s="8"/>
       <c r="Q100" t="b">
         <v>1</v>
@@ -5401,9 +5343,9 @@
       <c r="L101" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M101" s="17"/>
-      <c r="N101" s="17"/>
-      <c r="O101" s="17"/>
+      <c r="M101" s="15"/>
+      <c r="N101" s="15"/>
+      <c r="O101" s="15"/>
       <c r="P101" s="8"/>
       <c r="Q101" t="b">
         <v>1</v>
@@ -5450,9 +5392,9 @@
       <c r="L102" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M102" s="17"/>
-      <c r="N102" s="17"/>
-      <c r="O102" s="17"/>
+      <c r="M102" s="15"/>
+      <c r="N102" s="15"/>
+      <c r="O102" s="15"/>
       <c r="P102" s="8"/>
       <c r="Q102" t="b">
         <v>1</v>
@@ -5499,9 +5441,9 @@
       <c r="L103" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M103" s="17"/>
-      <c r="N103" s="17"/>
-      <c r="O103" s="17"/>
+      <c r="M103" s="15"/>
+      <c r="N103" s="15"/>
+      <c r="O103" s="15"/>
       <c r="P103" s="8"/>
       <c r="Q103" t="b">
         <v>1</v>
@@ -5545,9 +5487,9 @@
       <c r="L104" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M104" s="17"/>
-      <c r="N104" s="17"/>
-      <c r="O104" s="17"/>
+      <c r="M104" s="15"/>
+      <c r="N104" s="15"/>
+      <c r="O104" s="15"/>
       <c r="P104" s="8"/>
       <c r="Q104" t="b">
         <v>1</v>
@@ -5570,9 +5512,9 @@
       <c r="G105" s="6">
         <v>13.6</v>
       </c>
-      <c r="M105" s="17"/>
-      <c r="N105" s="17"/>
-      <c r="O105" s="17"/>
+      <c r="M105" s="15"/>
+      <c r="N105" s="15"/>
+      <c r="O105" s="15"/>
       <c r="P105" s="8"/>
       <c r="Q105" t="b">
         <v>1</v>
@@ -5585,6 +5527,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="N1:N2"/>
     <mergeCell ref="M95:O105"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="I1:I2"/>
@@ -5593,41 +5540,36 @@
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="M76:O88"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="N1:N2"/>
   </mergeCells>
   <conditionalFormatting sqref="R3:R35 R39:R74 R83 L33:L105 Q76:Q83">
-    <cfRule type="cellIs" dxfId="63" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="61" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="62" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R36:R38">
-    <cfRule type="cellIs" dxfId="61" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="59" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="60" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q95 Q97:Q99 Q101:Q104">
-    <cfRule type="cellIs" dxfId="59" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="57" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="58" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q13">
-    <cfRule type="cellIs" dxfId="53" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="52" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5784,10 +5726,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q86">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5799,8 +5741,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z105"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="U103" sqref="U103:V103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5814,55 +5757,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="15" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17" t="s">
+      <c r="M1" s="15"/>
+      <c r="N1" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17" t="s">
+      <c r="O1" s="15"/>
+      <c r="P1" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17" t="s">
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="S1" s="17" t="s">
+      <c r="S1" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="T1" s="18" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="2" t="s">
         <v>79</v>
       </c>
@@ -5881,19 +5824,19 @@
       <c r="G2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="20"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="18"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
@@ -5923,7 +5866,7 @@
       <c r="I3" s="7">
         <v>4.2809520330000002</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="21">
         <v>4.1970690258329197</v>
       </c>
       <c r="K3" s="7">
@@ -5990,7 +5933,7 @@
       <c r="I4" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K4" s="7">
@@ -6057,7 +6000,7 @@
       <c r="I5" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K5" s="7">
@@ -6124,7 +6067,7 @@
       <c r="I6" s="7">
         <v>4.2809520330000002</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="21">
         <v>4.1970690258329197</v>
       </c>
       <c r="K6" s="7">
@@ -6191,7 +6134,7 @@
       <c r="I7" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K7" s="7">
@@ -6258,7 +6201,7 @@
       <c r="I8" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K8" s="7">
@@ -6325,7 +6268,7 @@
       <c r="I9" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K9" s="7">
@@ -6392,7 +6335,7 @@
       <c r="I10" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K10" s="7">
@@ -6459,7 +6402,7 @@
       <c r="I11" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K11" s="7">
@@ -6526,7 +6469,7 @@
       <c r="I12" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K12" s="7">
@@ -6569,6 +6512,7 @@
       <c r="A13" s="14">
         <v>11</v>
       </c>
+      <c r="J13" s="21"/>
       <c r="R13"/>
       <c r="S13"/>
       <c r="T13" t="b">
@@ -6605,7 +6549,7 @@
       <c r="I14" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K14" s="7">
@@ -6672,7 +6616,7 @@
       <c r="I15" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K15" s="7">
@@ -6739,7 +6683,7 @@
       <c r="I16" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K16" s="7">
@@ -6806,7 +6750,7 @@
       <c r="I17" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="21">
         <v>1.4</v>
       </c>
       <c r="K17" s="7">
@@ -6873,7 +6817,7 @@
       <c r="I18" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="21">
         <v>1.4</v>
       </c>
       <c r="K18" s="7">
@@ -6940,7 +6884,7 @@
       <c r="I19" s="7">
         <v>4.2809520330000002</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="21">
         <v>1.2050000000000001</v>
       </c>
       <c r="K19" s="7">
@@ -7007,7 +6951,7 @@
       <c r="I20" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="21">
         <v>1.4</v>
       </c>
       <c r="K20" s="7">
@@ -7074,7 +7018,7 @@
       <c r="I21" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="21">
         <v>1.4</v>
       </c>
       <c r="K21" s="7">
@@ -7141,7 +7085,7 @@
       <c r="I22" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J22" s="7">
+      <c r="J22" s="21">
         <v>1.4</v>
       </c>
       <c r="K22" s="7">
@@ -7208,7 +7152,7 @@
       <c r="I23" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J23" s="7">
+      <c r="J23" s="21">
         <v>1.4</v>
       </c>
       <c r="K23" s="7">
@@ -7275,7 +7219,7 @@
       <c r="I24" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J24" s="7">
+      <c r="J24" s="21">
         <v>1.4</v>
       </c>
       <c r="K24" s="7">
@@ -7342,7 +7286,7 @@
       <c r="I25" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J25" s="7">
+      <c r="J25" s="21">
         <v>1.4</v>
       </c>
       <c r="K25" s="7">
@@ -7409,7 +7353,7 @@
       <c r="I26" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J26" s="7">
+      <c r="J26" s="21">
         <v>1.4</v>
       </c>
       <c r="K26" s="7">
@@ -7476,7 +7420,7 @@
       <c r="I27" s="7">
         <v>4.2809520330000002</v>
       </c>
-      <c r="J27" s="7">
+      <c r="J27" s="21">
         <v>1.2050000000000001</v>
       </c>
       <c r="K27" s="7">
@@ -7543,7 +7487,7 @@
       <c r="I28" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J28" s="7">
+      <c r="J28" s="21">
         <v>1.4</v>
       </c>
       <c r="K28" s="7">
@@ -7610,7 +7554,7 @@
       <c r="I29" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J29" s="7">
+      <c r="J29" s="21">
         <v>1.4</v>
       </c>
       <c r="K29" s="7">
@@ -7677,7 +7621,7 @@
       <c r="I30" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J30" s="7">
+      <c r="J30" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K30" s="7">
@@ -7744,7 +7688,7 @@
       <c r="I31" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J31" s="7">
+      <c r="J31" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K31" s="7">
@@ -7787,6 +7731,7 @@
       <c r="A32" s="14">
         <v>30</v>
       </c>
+      <c r="J32" s="21"/>
       <c r="R32"/>
       <c r="S32"/>
       <c r="T32" t="b">
@@ -7823,7 +7768,7 @@
       <c r="I33" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J33" s="7">
+      <c r="J33" s="21">
         <v>1.4</v>
       </c>
       <c r="K33" s="7">
@@ -7890,7 +7835,7 @@
       <c r="I34" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J34" s="7">
+      <c r="J34" s="21">
         <v>1.4</v>
       </c>
       <c r="K34" s="7">
@@ -7933,6 +7878,7 @@
       <c r="A35" s="14">
         <v>33</v>
       </c>
+      <c r="J35" s="21"/>
       <c r="R35"/>
       <c r="S35"/>
       <c r="T35" t="b">
@@ -7969,7 +7915,7 @@
       <c r="I36" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J36" s="7">
+      <c r="J36" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K36" s="7">
@@ -8036,7 +7982,7 @@
       <c r="I37" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J37" s="7">
+      <c r="J37" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K37" s="7">
@@ -8103,7 +8049,7 @@
       <c r="I38" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J38" s="7">
+      <c r="J38" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K38" s="7">
@@ -8170,7 +8116,7 @@
       <c r="I39" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J39" s="7">
+      <c r="J39" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K39" s="7">
@@ -8237,7 +8183,7 @@
       <c r="I40" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J40" s="7">
+      <c r="J40" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K40" s="7">
@@ -8304,7 +8250,7 @@
       <c r="I41" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J41" s="7">
+      <c r="J41" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K41" s="7">
@@ -8371,7 +8317,7 @@
       <c r="I42" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J42" s="7">
+      <c r="J42" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K42" s="7">
@@ -8438,7 +8384,7 @@
       <c r="I43" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J43" s="7">
+      <c r="J43" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K43" s="7">
@@ -8505,7 +8451,7 @@
       <c r="I44" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J44" s="7">
+      <c r="J44" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K44" s="7">
@@ -8572,7 +8518,7 @@
       <c r="I45" s="7">
         <v>4.2809520330000002</v>
       </c>
-      <c r="J45" s="7">
+      <c r="J45" s="21">
         <v>4.1970690258329197</v>
       </c>
       <c r="K45" s="7">
@@ -8615,6 +8561,7 @@
       <c r="A46" s="14">
         <v>44</v>
       </c>
+      <c r="J46" s="21"/>
       <c r="R46"/>
       <c r="S46"/>
       <c r="T46" t="b">
@@ -8627,6 +8574,7 @@
       <c r="A47" s="14">
         <v>45</v>
       </c>
+      <c r="J47" s="21"/>
       <c r="R47"/>
       <c r="S47"/>
       <c r="T47" t="b">
@@ -8639,6 +8587,7 @@
       <c r="A48" s="14">
         <v>46</v>
       </c>
+      <c r="J48" s="21"/>
       <c r="R48"/>
       <c r="S48"/>
       <c r="T48" t="b">
@@ -8651,6 +8600,7 @@
       <c r="A49" s="14">
         <v>47</v>
       </c>
+      <c r="J49" s="21"/>
       <c r="R49"/>
       <c r="S49"/>
       <c r="T49" t="b">
@@ -8663,6 +8613,7 @@
       <c r="A50" s="14">
         <v>48</v>
       </c>
+      <c r="J50" s="21"/>
       <c r="R50"/>
       <c r="S50"/>
       <c r="T50" t="b">
@@ -8699,7 +8650,7 @@
       <c r="I51" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J51" s="7">
+      <c r="J51" s="21">
         <v>1.4</v>
       </c>
       <c r="K51" s="7">
@@ -8742,6 +8693,7 @@
       <c r="A52" s="14">
         <v>50</v>
       </c>
+      <c r="J52" s="21"/>
       <c r="R52"/>
       <c r="S52"/>
       <c r="T52" t="b">
@@ -8754,6 +8706,7 @@
       <c r="A53" s="14">
         <v>51</v>
       </c>
+      <c r="J53" s="21"/>
       <c r="R53"/>
       <c r="S53"/>
       <c r="T53" t="b">
@@ -8766,6 +8719,7 @@
       <c r="A54" s="14">
         <v>52</v>
       </c>
+      <c r="J54" s="21"/>
       <c r="R54"/>
       <c r="S54"/>
       <c r="T54" t="b">
@@ -8778,6 +8732,7 @@
       <c r="A55" s="14">
         <v>53</v>
       </c>
+      <c r="J55" s="21"/>
       <c r="R55"/>
       <c r="S55"/>
       <c r="T55" t="b">
@@ -8790,6 +8745,7 @@
       <c r="A56" s="14">
         <v>54</v>
       </c>
+      <c r="J56" s="21"/>
       <c r="R56"/>
       <c r="S56"/>
       <c r="T56" t="b">
@@ -8802,6 +8758,7 @@
       <c r="A57" s="14">
         <v>55</v>
       </c>
+      <c r="J57" s="21"/>
       <c r="R57"/>
       <c r="S57"/>
       <c r="T57" t="b">
@@ -8814,6 +8771,7 @@
       <c r="A58" s="14">
         <v>56</v>
       </c>
+      <c r="J58" s="21"/>
       <c r="R58"/>
       <c r="S58"/>
       <c r="T58" t="b">
@@ -8850,7 +8808,7 @@
       <c r="I59" s="7">
         <v>4.2809520330000002</v>
       </c>
-      <c r="J59" s="7">
+      <c r="J59" s="21">
         <v>4.1970690258329197</v>
       </c>
       <c r="K59" s="7">
@@ -8917,7 +8875,7 @@
       <c r="I60" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J60" s="7">
+      <c r="J60" s="21">
         <v>1.4</v>
       </c>
       <c r="K60" s="7">
@@ -8984,7 +8942,7 @@
       <c r="I61" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J61" s="7">
+      <c r="J61" s="21">
         <v>1.4</v>
       </c>
       <c r="K61" s="7">
@@ -9051,7 +9009,7 @@
       <c r="I62" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J62" s="7">
+      <c r="J62" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K62" s="7">
@@ -9118,7 +9076,7 @@
       <c r="I63" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J63" s="7">
+      <c r="J63" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K63" s="7">
@@ -9185,7 +9143,7 @@
       <c r="I64" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J64" s="7">
+      <c r="J64" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K64" s="7">
@@ -9228,6 +9186,7 @@
       <c r="A65" s="14">
         <v>63</v>
       </c>
+      <c r="J65" s="21"/>
       <c r="R65"/>
       <c r="S65"/>
       <c r="T65" t="b">
@@ -9264,7 +9223,7 @@
       <c r="I66" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J66" s="7">
+      <c r="J66" s="21">
         <v>1.4</v>
       </c>
       <c r="K66" s="7">
@@ -9331,7 +9290,7 @@
       <c r="I67" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J67" s="7">
+      <c r="J67" s="21">
         <v>1.4</v>
       </c>
       <c r="K67" s="7">
@@ -9398,7 +9357,7 @@
       <c r="I68" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J68" s="7">
+      <c r="J68" s="21">
         <v>1.4</v>
       </c>
       <c r="K68" s="7">
@@ -9465,7 +9424,7 @@
       <c r="I69" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J69" s="7">
+      <c r="J69" s="21">
         <v>1.4</v>
       </c>
       <c r="K69" s="7">
@@ -9532,7 +9491,7 @@
       <c r="I70" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J70" s="7">
+      <c r="J70" s="21">
         <v>1.4</v>
       </c>
       <c r="K70" s="7">
@@ -9599,7 +9558,7 @@
       <c r="I71" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J71" s="7">
+      <c r="J71" s="21">
         <v>1.4</v>
       </c>
       <c r="K71" s="7">
@@ -9666,7 +9625,7 @@
       <c r="I72" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J72" s="7">
+      <c r="J72" s="21">
         <v>1.4</v>
       </c>
       <c r="K72" s="7">
@@ -9733,7 +9692,7 @@
       <c r="I73" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J73" s="7">
+      <c r="J73" s="21">
         <v>1.4</v>
       </c>
       <c r="K73" s="7">
@@ -9800,7 +9759,7 @@
       <c r="I74" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J74" s="7">
+      <c r="J74" s="21">
         <v>1.4</v>
       </c>
       <c r="K74" s="7">
@@ -9867,7 +9826,7 @@
       <c r="I75" s="7">
         <v>2.7953305990000001</v>
       </c>
-      <c r="J75" s="7">
+      <c r="J75" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K75" s="7">
@@ -9934,7 +9893,7 @@
       <c r="I76" s="7">
         <v>2.818100115</v>
       </c>
-      <c r="J76" s="7">
+      <c r="J76" s="21">
         <v>0</v>
       </c>
       <c r="K76" s="7">
@@ -9977,6 +9936,7 @@
       <c r="A77" s="14">
         <v>75</v>
       </c>
+      <c r="J77" s="21"/>
       <c r="R77"/>
       <c r="S77"/>
       <c r="T77" t="b">
@@ -10013,7 +9973,7 @@
       <c r="I78" s="7">
         <v>2.818100115</v>
       </c>
-      <c r="J78" s="7">
+      <c r="J78" s="21">
         <v>0</v>
       </c>
       <c r="K78" s="7">
@@ -10080,7 +10040,7 @@
       <c r="I79" s="7">
         <v>1.4098211549999999</v>
       </c>
-      <c r="J79" s="7">
+      <c r="J79" s="21">
         <v>0</v>
       </c>
       <c r="K79" s="7">
@@ -10147,7 +10107,7 @@
       <c r="I80" s="7">
         <v>2.818100115</v>
       </c>
-      <c r="J80" s="7">
+      <c r="J80" s="21">
         <v>0</v>
       </c>
       <c r="K80" s="7">
@@ -10190,6 +10150,7 @@
       <c r="A81" s="14">
         <v>79</v>
       </c>
+      <c r="J81" s="21"/>
       <c r="R81"/>
       <c r="S81"/>
       <c r="T81" t="b">
@@ -10226,7 +10187,7 @@
       <c r="I82" s="7">
         <v>2.818100115</v>
       </c>
-      <c r="J82" s="7">
+      <c r="J82" s="21">
         <v>0</v>
       </c>
       <c r="K82" s="7">
@@ -10293,7 +10254,7 @@
       <c r="I83" s="7">
         <v>1.4098211549999999</v>
       </c>
-      <c r="J83" s="7">
+      <c r="J83" s="21">
         <v>0</v>
       </c>
       <c r="K83" s="7">
@@ -10360,7 +10321,7 @@
       <c r="I84" s="7">
         <v>1.4098211549999999</v>
       </c>
-      <c r="J84" s="7">
+      <c r="J84" s="21">
         <v>0</v>
       </c>
       <c r="K84" s="7">
@@ -10427,7 +10388,7 @@
       <c r="I85" s="7">
         <v>2.818100115</v>
       </c>
-      <c r="J85" s="7">
+      <c r="J85" s="21">
         <v>0</v>
       </c>
       <c r="K85" s="7">
@@ -10470,6 +10431,7 @@
       <c r="A86" s="14">
         <v>84</v>
       </c>
+      <c r="J86" s="21"/>
       <c r="R86"/>
       <c r="S86"/>
       <c r="T86" t="b">
@@ -10506,7 +10468,7 @@
       <c r="I87" s="7">
         <v>2.818100115</v>
       </c>
-      <c r="J87" s="7">
+      <c r="J87" s="21">
         <v>0</v>
       </c>
       <c r="K87" s="7">
@@ -10573,7 +10535,7 @@
       <c r="I88" s="7">
         <v>1.4098211549999999</v>
       </c>
-      <c r="J88" s="7">
+      <c r="J88" s="21">
         <v>0</v>
       </c>
       <c r="K88" s="7">
@@ -10640,7 +10602,7 @@
       <c r="I89" s="2">
         <v>2.818100115</v>
       </c>
-      <c r="J89" s="2">
+      <c r="J89" s="21">
         <v>1.4</v>
       </c>
       <c r="K89" s="2">
@@ -10702,7 +10664,7 @@
       <c r="I90" s="2">
         <v>2.8555274160000002</v>
       </c>
-      <c r="J90" s="2">
+      <c r="J90" s="21">
         <v>1.4</v>
       </c>
       <c r="K90" s="2">
@@ -10764,7 +10726,7 @@
       <c r="I91" s="2">
         <v>2.818100115</v>
       </c>
-      <c r="J91" s="2">
+      <c r="J91" s="21">
         <v>1.4</v>
       </c>
       <c r="K91" s="2">
@@ -10826,7 +10788,7 @@
       <c r="I92" s="2">
         <v>1.4098211549999999</v>
       </c>
-      <c r="J92" s="2">
+      <c r="J92" s="21">
         <v>1.4</v>
       </c>
       <c r="K92" s="2">
@@ -10888,7 +10850,7 @@
       <c r="I93" s="2">
         <v>1.4098211549999999</v>
       </c>
-      <c r="J93" s="2">
+      <c r="J93" s="21">
         <v>1.4</v>
       </c>
       <c r="K93" s="2">
@@ -10950,7 +10912,7 @@
       <c r="I94" s="2">
         <v>35.081892850000003</v>
       </c>
-      <c r="J94" s="2">
+      <c r="J94" s="21">
         <v>2.7637067034554601</v>
       </c>
       <c r="K94" s="2">
@@ -11012,7 +10974,7 @@
       <c r="I95" s="2">
         <v>34.6230908</v>
       </c>
-      <c r="J95" s="2">
+      <c r="J95" s="21">
         <v>0</v>
       </c>
       <c r="K95" s="2">
@@ -11065,7 +11027,7 @@
       </c>
       <c r="H96" s="14"/>
       <c r="I96" s="14"/>
-      <c r="J96" s="13"/>
+      <c r="J96" s="22"/>
       <c r="K96" s="13"/>
       <c r="T96" s="2" t="b">
         <v>1</v>
@@ -11102,7 +11064,7 @@
         <v>59</v>
       </c>
       <c r="I97" s="14"/>
-      <c r="J97" s="13"/>
+      <c r="J97" s="22"/>
       <c r="K97" s="13"/>
       <c r="T97" s="14" t="b">
         <v>1</v>
@@ -11139,7 +11101,7 @@
         <v>60</v>
       </c>
       <c r="I98" s="14"/>
-      <c r="J98" s="13"/>
+      <c r="J98" s="22"/>
       <c r="K98" s="13"/>
       <c r="T98" s="14" t="b">
         <v>1</v>
@@ -11176,7 +11138,7 @@
         <v>61</v>
       </c>
       <c r="I99" s="14"/>
-      <c r="J99" s="13"/>
+      <c r="J99" s="22"/>
       <c r="K99" s="13"/>
       <c r="T99" s="14" t="b">
         <v>1</v>
@@ -11205,7 +11167,7 @@
       </c>
       <c r="H100" s="14"/>
       <c r="I100" s="14"/>
-      <c r="J100" s="13"/>
+      <c r="J100" s="22"/>
       <c r="K100" s="13"/>
       <c r="T100" s="14" t="b">
         <v>1</v>
@@ -11242,7 +11204,7 @@
         <v>62</v>
       </c>
       <c r="I101" s="14"/>
-      <c r="J101" s="13"/>
+      <c r="J101" s="22"/>
       <c r="K101" s="13"/>
       <c r="T101" s="14" t="b">
         <v>1</v>
@@ -11279,7 +11241,7 @@
         <v>63</v>
       </c>
       <c r="I102" s="14"/>
-      <c r="J102" s="13"/>
+      <c r="J102" s="22"/>
       <c r="K102" s="13"/>
       <c r="T102" s="14" t="b">
         <v>1</v>
@@ -11316,7 +11278,7 @@
         <v>64</v>
       </c>
       <c r="I103" s="14"/>
-      <c r="J103" s="13"/>
+      <c r="J103" s="22"/>
       <c r="K103" s="13"/>
       <c r="T103" s="14" t="b">
         <v>1</v>
@@ -11353,7 +11315,7 @@
         <v>65</v>
       </c>
       <c r="I104" s="14"/>
-      <c r="J104" s="13"/>
+      <c r="J104" s="22"/>
       <c r="K104" s="13"/>
       <c r="T104" s="14" t="b">
         <v>1</v>
@@ -11363,7 +11325,7 @@
       <c r="Y104"/>
       <c r="Z104" s="2"/>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="14">
         <f t="shared" si="10"/>
         <v>103</v>
@@ -11382,7 +11344,7 @@
       </c>
       <c r="H105" s="14"/>
       <c r="I105" s="14"/>
-      <c r="J105" s="13"/>
+      <c r="J105" s="23"/>
       <c r="K105" s="13"/>
       <c r="T105" s="14" t="b">
         <v>1</v>
@@ -11394,6 +11356,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:M2"/>
@@ -11401,42 +11369,36 @@
     <mergeCell ref="P1:Q2"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="S1:S2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="V3:V95">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:S95">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:T95">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R95">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>